<commit_message>
Sequence of questions done
</commit_message>
<xml_diff>
--- a/FM-Visualization/FMsAllSpec.xlsx
+++ b/FM-Visualization/FMsAllSpec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\Projects\Eye-Tracking-VariableSytems\R-Repository\R-repository\FM-Visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32B171C-4521-4C3E-BBD0-2DE62F2BF20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A3C92E-B469-4C4B-A6A7-AEF5D28DEB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49980" yWindow="1215" windowWidth="19950" windowHeight="14415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47880" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FMsAllSpec" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="85">
   <si>
     <t>No.Features</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>Revised - New mapping</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>New</t>
   </si>
 </sst>
 </file>
@@ -614,7 +620,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -759,6 +765,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -806,13 +838,19 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="1" fillId="33" borderId="11" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1972,10 +2010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD453E1-7F15-49AA-9A64-D0BF03A6D5EF}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="J21" sqref="J21:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2155,17 +2193,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.5">
       <c r="C17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.5">
       <c r="C18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.5">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.5">
       <c r="C19" t="s">
         <v>68</v>
       </c>
@@ -2173,93 +2211,115 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.5">
-      <c r="H21" t="s">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.5">
+      <c r="H21" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="K21" t="s">
+      <c r="I21" s="5"/>
+      <c r="J21" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.5">
-      <c r="H22" t="s">
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.5">
+      <c r="H22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.5">
+      <c r="H23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K22" t="s">
+      <c r="J23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L22" t="s">
+      <c r="K23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.5">
-      <c r="H23" t="s">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.5">
+      <c r="H24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K23" t="s">
+      <c r="J24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L23" t="s">
+      <c r="K24" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.5">
-      <c r="H24" t="s">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.5">
+      <c r="H25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K24" t="s">
+      <c r="J25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L24" t="s">
+      <c r="K25" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.5">
-      <c r="H25" t="s">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.5">
+      <c r="H26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K25" t="s">
+      <c r="J26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L25" t="s">
+      <c r="K26" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.5">
-      <c r="H26" t="s">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.5">
+      <c r="H27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K26" t="s">
+      <c r="J27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L26" t="s">
+      <c r="K27" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.5">
-      <c r="K27" t="s">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.5">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L27" t="s">
+      <c r="K28" s="2" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>